<commit_message>
Changed : to = to denote column value
</commit_message>
<xml_diff>
--- a/packages/ambre/tests/actual_expected/rule_extraction_titanic.expected.xlsx
+++ b/packages/ambre/tests/actual_expected/rule_extraction_titanic.expected.xlsx
@@ -474,12 +474,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>parch:0 ∪ pclass:1 ∪ sex:female</t>
+          <t>parch=0 ∪ pclass=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -501,12 +501,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pclass:1 ∪ sex:female ∪ sibsp:0</t>
+          <t>pclass=1 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -528,12 +528,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>embarked:c ∪ pclass:1 ∪ sex:female</t>
+          <t>embarked=c ∪ pclass=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -555,12 +555,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>parch:0 ∪ pclass:1 ∪ sex:female ∪ sibsp:0</t>
+          <t>parch=0 ∪ pclass=1 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -582,12 +582,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>embarked:c ∪ parch:0 ∪ pclass:1 ∪ sex:female</t>
+          <t>embarked=c ∪ parch=0 ∪ pclass=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -609,12 +609,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pclass:1 ∪ sex:female</t>
+          <t>pclass=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -636,12 +636,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>embarked:s ∪ pclass:1 ∪ sex:female</t>
+          <t>embarked=s ∪ pclass=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -663,12 +663,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>pclass:1 ∪ sex:female ∪ sibsp:1</t>
+          <t>pclass=1 ∪ sex=female ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -690,12 +690,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pclass:2 ∪ sex:female ∪ sibsp:0</t>
+          <t>pclass=2 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -717,12 +717,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>embarked:s ∪ pclass:2 ∪ sex:female ∪ sibsp:0</t>
+          <t>embarked=s ∪ pclass=2 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -744,12 +744,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>pclass:2 ∪ sex:female</t>
+          <t>pclass=2 ∪ sex=female</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -771,12 +771,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>embarked:s ∪ pclass:2 ∪ sex:female</t>
+          <t>embarked=s ∪ pclass=2 ∪ sex=female</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -798,12 +798,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>embarked:c ∪ parch:0 ∪ sex:female</t>
+          <t>embarked=c ∪ parch=0 ∪ sex=female</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -825,12 +825,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>parch:0 ∪ pclass:2 ∪ sex:female</t>
+          <t>parch=0 ∪ pclass=2 ∪ sex=female</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -852,12 +852,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>embarked:c ∪ sex:female</t>
+          <t>embarked=c ∪ sex=female</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -879,12 +879,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>embarked:c ∪ sex:female ∪ sibsp:0</t>
+          <t>embarked=c ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -906,12 +906,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>embarked:s ∪ parch:0 ∪ pclass:2 ∪ sex:female</t>
+          <t>embarked=s ∪ parch=0 ∪ pclass=2 ∪ sex=female</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -933,12 +933,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>age:nan ∪ parch:0 ∪ sex:female</t>
+          <t>age=nan ∪ parch=0 ∪ sex=female</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -960,12 +960,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>parch:0 ∪ sex:female ∪ sibsp:1</t>
+          <t>parch=0 ∪ sex=female ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -987,12 +987,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>parch:0 ∪ sex:female</t>
+          <t>parch=0 ∪ sex=female</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1014,12 +1014,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>sex:female ∪ sibsp:0</t>
+          <t>sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1041,12 +1041,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>parch:0 ∪ sex:female ∪ sibsp:0</t>
+          <t>parch=0 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1068,12 +1068,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>embarked:s ∪ parch:1 ∪ sex:female</t>
+          <t>embarked=s ∪ parch=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1095,12 +1095,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>embarked:s ∪ sex:female ∪ sibsp:0</t>
+          <t>embarked=s ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1122,12 +1122,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>parch:1 ∪ sex:female</t>
+          <t>parch=1 ∪ sex=female</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1149,12 +1149,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>parch:0 ∪ pclass:1 ∪ sibsp:1</t>
+          <t>parch=0 ∪ pclass=1 ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1176,12 +1176,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>sex:female ∪ sibsp:1</t>
+          <t>sex=female ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1203,12 +1203,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>pclass:1 ∪ sibsp:1</t>
+          <t>pclass=1 ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1230,12 +1230,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>sex:female</t>
+          <t>sex=female</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1257,12 +1257,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>embarked:s ∪ parch:0 ∪ sex:female ∪ sibsp:0</t>
+          <t>embarked=s ∪ parch=0 ∪ sex=female ∪ sibsp=0</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1284,12 +1284,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>embarked:s ∪ parch:0 ∪ sex:female</t>
+          <t>embarked=s ∪ parch=0 ∪ sex=female</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1311,12 +1311,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>embarked:c ∪ parch:0 ∪ pclass:1</t>
+          <t>embarked=c ∪ parch=0 ∪ pclass=1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1338,12 +1338,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>embarked:s ∪ sex:female ∪ sibsp:1</t>
+          <t>embarked=s ∪ sex=female ∪ sibsp=1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>survived:1</t>
+          <t>survived=1</t>
         </is>
       </c>
       <c r="C34" t="n">

</xml_diff>

<commit_message>
Added consequents_length to rule extraction
</commit_message>
<xml_diff>
--- a/packages/ambre/tests/actual_expected/rule_extraction_titanic.expected.xlsx
+++ b/packages/ambre/tests/actual_expected/rule_extraction_titanic.expected.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,21 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +469,11 @@
           <t>antecedents_length</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>consequents_length</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -497,6 +501,9 @@
       <c r="G2" t="n">
         <v>3</v>
       </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -524,6 +531,9 @@
       <c r="G3" t="n">
         <v>3</v>
       </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -551,6 +561,9 @@
       <c r="G4" t="n">
         <v>3</v>
       </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -578,6 +591,9 @@
       <c r="G5" t="n">
         <v>4</v>
       </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -605,6 +621,9 @@
       <c r="G6" t="n">
         <v>4</v>
       </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -632,6 +651,9 @@
       <c r="G7" t="n">
         <v>2</v>
       </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -659,6 +681,9 @@
       <c r="G8" t="n">
         <v>3</v>
       </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -686,6 +711,9 @@
       <c r="G9" t="n">
         <v>3</v>
       </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -713,6 +741,9 @@
       <c r="G10" t="n">
         <v>3</v>
       </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -740,6 +771,9 @@
       <c r="G11" t="n">
         <v>4</v>
       </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -767,6 +801,9 @@
       <c r="G12" t="n">
         <v>2</v>
       </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -794,6 +831,9 @@
       <c r="G13" t="n">
         <v>3</v>
       </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -821,6 +861,9 @@
       <c r="G14" t="n">
         <v>3</v>
       </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -848,6 +891,9 @@
       <c r="G15" t="n">
         <v>3</v>
       </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -875,6 +921,9 @@
       <c r="G16" t="n">
         <v>2</v>
       </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -902,6 +951,9 @@
       <c r="G17" t="n">
         <v>3</v>
       </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -929,6 +981,9 @@
       <c r="G18" t="n">
         <v>4</v>
       </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -956,6 +1011,9 @@
       <c r="G19" t="n">
         <v>3</v>
       </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -983,6 +1041,9 @@
       <c r="G20" t="n">
         <v>3</v>
       </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1010,6 +1071,9 @@
       <c r="G21" t="n">
         <v>2</v>
       </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1037,6 +1101,9 @@
       <c r="G22" t="n">
         <v>2</v>
       </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1064,6 +1131,9 @@
       <c r="G23" t="n">
         <v>3</v>
       </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1091,6 +1161,9 @@
       <c r="G24" t="n">
         <v>3</v>
       </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1118,6 +1191,9 @@
       <c r="G25" t="n">
         <v>3</v>
       </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1145,6 +1221,9 @@
       <c r="G26" t="n">
         <v>2</v>
       </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1172,6 +1251,9 @@
       <c r="G27" t="n">
         <v>3</v>
       </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1199,6 +1281,9 @@
       <c r="G28" t="n">
         <v>2</v>
       </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1226,6 +1311,9 @@
       <c r="G29" t="n">
         <v>2</v>
       </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1253,6 +1341,9 @@
       <c r="G30" t="n">
         <v>1</v>
       </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1280,6 +1371,9 @@
       <c r="G31" t="n">
         <v>4</v>
       </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1307,6 +1401,9 @@
       <c r="G32" t="n">
         <v>3</v>
       </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1334,6 +1431,9 @@
       <c r="G33" t="n">
         <v>3</v>
       </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1361,8 +1461,11 @@
       <c r="G34" t="n">
         <v>3</v>
       </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>